<commit_message>
updated with aragonite saturation state
</commit_message>
<xml_diff>
--- a/2016-17_PteropodExp_WaterChem/PteropodWaterChem/Table_1.xlsx
+++ b/2016-17_PteropodExp_WaterChem/PteropodWaterChem/Table_1.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Shelly/Documents/GitHub/Seawater-Chemistry-Analysis/2016-17_PteropodExp_WaterChem/PteropodWaterChem/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D198D527-A1FB-7F42-9216-D01119452885}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F49A2BDE-56F0-084E-9176-433D18D96026}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4960" yWindow="1560" windowWidth="20420" windowHeight="14140" xr2:uid="{C34F0D06-2772-1442-BC30-9EB6600E88F0}"/>
+    <workbookView xWindow="12380" yWindow="1240" windowWidth="20420" windowHeight="14140" xr2:uid="{C34F0D06-2772-1442-BC30-9EB6600E88F0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -31,40 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="22">
-  <si>
-    <t>treatment</t>
-  </si>
-  <si>
-    <t>target pH</t>
-  </si>
-  <si>
-    <t>Spectrophotometric pH</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Logger pH </t>
-  </si>
-  <si>
-    <t>ambient pH ambient DO</t>
-  </si>
-  <si>
-    <t>ambient pH low DO</t>
-  </si>
-  <si>
-    <t>low pH ambient DO</t>
-  </si>
-  <si>
-    <t>low pH low DO</t>
-  </si>
-  <si>
-    <t>salinity</t>
-  </si>
-  <si>
-    <t>29.62 psu (from spec data and PMEL data (29.61psu))</t>
-  </si>
-  <si>
-    <t>manuscript draft says avg salinity was 28.94psu, but not sure how this was calculated or what the raw data was</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="37">
   <si>
     <t>TA</t>
   </si>
@@ -84,19 +51,97 @@
     <t>Logger DO (mg/L)</t>
   </si>
   <si>
-    <t>3.73 +/- 0.43</t>
-  </si>
-  <si>
-    <t>9.22 +/- 0.13</t>
-  </si>
-  <si>
-    <t>9.31 +/- 0.15</t>
-  </si>
-  <si>
-    <t>7.54 +/- 0.04</t>
-  </si>
-  <si>
     <t>7.87 +/- 0.03</t>
+  </si>
+  <si>
+    <t>9.31 +/- 0.16</t>
+  </si>
+  <si>
+    <t>3.73 +/- 0.42</t>
+  </si>
+  <si>
+    <t>9.23 +/- 0.12</t>
+  </si>
+  <si>
+    <t>Presens DO (mg/L)</t>
+  </si>
+  <si>
+    <t>7.91 +/- 0.02</t>
+  </si>
+  <si>
+    <t>7.94 +/- 0.02</t>
+  </si>
+  <si>
+    <t>7.55 +/- 0.03</t>
+  </si>
+  <si>
+    <t>7.56 +/- 0.03</t>
+  </si>
+  <si>
+    <t>7.87 +/- 0.05</t>
+  </si>
+  <si>
+    <t>7.53 +/- 0.03</t>
+  </si>
+  <si>
+    <t>7.55 +/- 0.05</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Logger pH (NBS) </t>
+  </si>
+  <si>
+    <t>Spectrophotometric pH (total scale)</t>
+  </si>
+  <si>
+    <t>1.11 +/- 0.11</t>
+  </si>
+  <si>
+    <t>1.11 +/- 0.07</t>
+  </si>
+  <si>
+    <t>0.53 +/- 0.04</t>
+  </si>
+  <si>
+    <t>0.56 +/- 0.06</t>
+  </si>
+  <si>
+    <t>9.42 +/- 0.22</t>
+  </si>
+  <si>
+    <t>3.86 +/- 0.64</t>
+  </si>
+  <si>
+    <t>9.85 +/- 0.07</t>
+  </si>
+  <si>
+    <t>3.64 +/- 0.12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">28.94 +/- 0.95 psu </t>
+  </si>
+  <si>
+    <t>Aragonite Saturation (Ω)</t>
+  </si>
+  <si>
+    <t>Target pH</t>
+  </si>
+  <si>
+    <t>Treatment</t>
+  </si>
+  <si>
+    <t>ambient pH + ambient DO</t>
+  </si>
+  <si>
+    <t>ambient pH + low DO</t>
+  </si>
+  <si>
+    <t>low pH + ambient DO</t>
+  </si>
+  <si>
+    <t>low pH + low DO</t>
+  </si>
+  <si>
+    <t>Salinity</t>
   </si>
 </sst>
 </file>
@@ -155,10 +200,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -475,140 +528,179 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{884E99F1-6715-6B4A-BE9C-E53F6E1A7C65}">
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:H9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" zoomScale="96" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5:H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="20.83203125" customWidth="1"/>
-    <col min="4" max="4" width="21.6640625" customWidth="1"/>
-    <col min="5" max="5" width="17.5" customWidth="1"/>
+    <col min="1" max="1" width="23.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="32.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="17.33203125" customWidth="1"/>
+    <col min="7" max="7" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B6" s="3">
+        <v>7.95</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="F6" s="3">
+        <v>9.32</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A7" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B7" s="3">
+        <v>7.95</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="F7" s="3">
+        <v>3.73</v>
+      </c>
+      <c r="G7" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B1" t="s">
+      <c r="H7" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A8" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B8" s="3">
+        <v>7.55</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="F8" s="3">
+        <v>9.32</v>
+      </c>
+      <c r="G8" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="F1" t="s">
-        <v>10</v>
+      <c r="H8" s="4" t="s">
+        <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B3" t="s">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A9" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B9" s="3">
+        <v>7.55</v>
+      </c>
+      <c r="C9" s="3" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A5" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" s="1">
-        <v>7.95</v>
-      </c>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E6" s="1">
-        <v>9.32</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A7" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B7" s="1">
-        <v>7.95</v>
-      </c>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E7" s="1">
+      <c r="D9" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F9" s="3">
         <v>3.73</v>
       </c>
-      <c r="F7" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A8" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B8" s="1">
-        <v>7.55</v>
-      </c>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E8" s="1">
-        <v>9.32</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A9" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B9" s="1">
-        <v>7.55</v>
-      </c>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E9" s="1">
-        <v>3.73</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>17</v>
+      <c r="G9" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="H9" s="4" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>